<commit_message>
fix: change the regex match
</commit_message>
<xml_diff>
--- a/original.xlsx
+++ b/original.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="14680" activeTab="2"/>
+    <workbookView windowWidth="14430" windowHeight="8227" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>名称</t>
   </si>
@@ -67,6 +69,120 @@
   </si>
   <si>
     <t>入职年限</t>
+  </si>
+  <si>
+    <t>姓名</t>
+  </si>
+  <si>
+    <t>日末余额</t>
+  </si>
+  <si>
+    <t>张  飞</t>
+  </si>
+  <si>
+    <t>张朝春</t>
+  </si>
+  <si>
+    <t>张成雷</t>
+  </si>
+  <si>
+    <t>张定芳</t>
+  </si>
+  <si>
+    <t>张和平</t>
+  </si>
+  <si>
+    <t>张洪平</t>
+  </si>
+  <si>
+    <t>张建忠</t>
+  </si>
+  <si>
+    <t>张金常</t>
+  </si>
+  <si>
+    <t>张连峰</t>
+  </si>
+  <si>
+    <t>张林</t>
+  </si>
+  <si>
+    <t>张强</t>
+  </si>
+  <si>
+    <t>张升云</t>
+  </si>
+  <si>
+    <t>张素文（餐饮会员）</t>
+  </si>
+  <si>
+    <t>张伟</t>
+  </si>
+  <si>
+    <t>张相富</t>
+  </si>
+  <si>
+    <t>张小红</t>
+  </si>
+  <si>
+    <t>张小平</t>
+  </si>
+  <si>
+    <t>张雪平（餐饮会员）</t>
+  </si>
+  <si>
+    <t>张燕丽</t>
+  </si>
+  <si>
+    <t>张毅</t>
+  </si>
+  <si>
+    <t>张瑜</t>
+  </si>
+  <si>
+    <t>张志刚</t>
+  </si>
+  <si>
+    <t>张中华</t>
+  </si>
+  <si>
+    <t>张  伟13388175520</t>
+  </si>
+  <si>
+    <t>张  瑜13550102799</t>
+  </si>
+  <si>
+    <t>张  飞13981965643</t>
+  </si>
+  <si>
+    <t>张中华13995123882</t>
+  </si>
+  <si>
+    <t>张升云18980219933</t>
+  </si>
+  <si>
+    <t>张和平13989005923</t>
+  </si>
+  <si>
+    <t>张定芳13801536028</t>
+  </si>
+  <si>
+    <t>张小平18982473897</t>
+  </si>
+  <si>
+    <t>张小红13893403941</t>
+  </si>
+  <si>
+    <t>张建忠18980596999</t>
+  </si>
+  <si>
+    <t>张成雷13198026666</t>
+  </si>
+  <si>
+    <t>张朝春18982166666</t>
+  </si>
+  <si>
+    <t>张毅13316094116</t>
   </si>
 </sst>
 </file>
@@ -79,19 +195,48 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="63"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="61"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="0"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -99,14 +244,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -114,7 +259,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -122,7 +267,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -130,7 +275,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -138,7 +283,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -146,14 +291,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -161,7 +306,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -169,7 +314,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -177,14 +322,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -192,42 +337,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -426,12 +571,51 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="63"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -552,191 +736,216 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -1217,7 +1426,7 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1290,9 +1499,9 @@
       <selection activeCell="A1" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="17.4453125" customWidth="1"/>
+    <col min="1" max="1" width="17.4424778761062" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1362,11 +1571,11 @@
   <sheetPr/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1422,6 +1631,356 @@
       </c>
       <c r="D4" t="s">
         <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="35.2566371681416" customWidth="1"/>
+    <col min="2" max="2" width="15.5398230088496" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7">
+        <v>2693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="6">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2920</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2920</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6">
+        <v>279.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="6">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="7">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="14" ht="38.25" spans="1:2">
+      <c r="A14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="6">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="6">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="6">
+        <v>924.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="6">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="19" ht="38.25" spans="1:2">
+      <c r="A19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="6">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="21.4424778761062" customWidth="1"/>
+    <col min="2" max="2" width="13.4159292035398" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" ht="33.75" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3">
+        <v>-152</v>
+      </c>
+    </row>
+    <row r="3" ht="33.75" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="3">
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="4" ht="33.75" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-308</v>
+      </c>
+    </row>
+    <row r="5" ht="33.75" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3">
+        <v>-152</v>
+      </c>
+    </row>
+    <row r="6" ht="33.75" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="3">
+        <v>-1573</v>
+      </c>
+    </row>
+    <row r="7" ht="33.75" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="3">
+        <v>-2920</v>
+      </c>
+    </row>
+    <row r="8" ht="33.75" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="3">
+        <v>-2920</v>
+      </c>
+    </row>
+    <row r="9" ht="33.75" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="3">
+        <v>-688</v>
+      </c>
+    </row>
+    <row r="10" ht="33.75" spans="1:2">
+      <c r="A10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3">
+        <v>-924.4</v>
+      </c>
+    </row>
+    <row r="11" ht="33.75" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="3">
+        <v>-1013</v>
+      </c>
+    </row>
+    <row r="12" ht="33.75" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="3">
+        <v>-360</v>
+      </c>
+    </row>
+    <row r="13" ht="33.75" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-2693</v>
+      </c>
+    </row>
+    <row r="14" ht="33.75" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="3">
+        <v>-1286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed: fix some known issues
</commit_message>
<xml_diff>
--- a/original.xlsx
+++ b/original.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14430" windowHeight="8227" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="12380" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <t>日末余额</t>
   </si>
   <si>
-    <t>张  飞</t>
+    <t>张  飞+</t>
   </si>
   <si>
     <t>张朝春</t>
@@ -199,7 +199,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -236,7 +236,7 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -244,14 +244,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -259,7 +259,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -267,7 +267,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -275,7 +275,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -283,7 +283,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -291,14 +291,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -306,7 +306,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -314,7 +314,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -322,14 +322,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -337,42 +337,42 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -897,55 +897,55 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -1426,7 +1426,7 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1499,9 +1499,9 @@
       <selection activeCell="A1" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="17.4424778761062" customWidth="1"/>
+    <col min="1" max="1" width="17.4453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1575,7 +1575,7 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1644,14 +1644,14 @@
   <sheetPr/>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.0234375" defaultRowHeight="16.8" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="35.2566371681416" customWidth="1"/>
-    <col min="2" max="2" width="15.5398230088496" customWidth="1"/>
+    <col min="1" max="1" width="35.2578125" customWidth="1"/>
+    <col min="2" max="2" width="15.5390625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1758,7 +1758,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="14" ht="38.25" spans="1:2">
+    <row r="14" spans="1:2">
       <c r="A14" s="5" t="s">
         <v>31</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="19" ht="38.25" spans="1:2">
+    <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
@@ -1861,14 +1861,14 @@
   <sheetPr/>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.0234375" defaultRowHeight="16.8" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="21.4424778761062" customWidth="1"/>
-    <col min="2" max="2" width="13.4159292035398" customWidth="1"/>
+    <col min="1" max="1" width="21.4453125" customWidth="1"/>
+    <col min="2" max="2" width="13.4140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1879,7 +1879,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="33.75" spans="1:2">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>-152</v>
       </c>
     </row>
-    <row r="3" ht="33.75" spans="1:2">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>-2000</v>
       </c>
     </row>
-    <row r="4" ht="33.75" spans="1:2">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>-308</v>
       </c>
     </row>
-    <row r="5" ht="33.75" spans="1:2">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>-152</v>
       </c>
     </row>
-    <row r="6" ht="33.75" spans="1:2">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>46</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>-1573</v>
       </c>
     </row>
-    <row r="7" ht="33.75" spans="1:2">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>-2920</v>
       </c>
     </row>
-    <row r="8" ht="33.75" spans="1:2">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>-2920</v>
       </c>
     </row>
-    <row r="9" ht="33.75" spans="1:2">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>49</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>-688</v>
       </c>
     </row>
-    <row r="10" ht="33.75" spans="1:2">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>-924.4</v>
       </c>
     </row>
-    <row r="11" ht="33.75" spans="1:2">
+    <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>-1013</v>
       </c>
     </row>
-    <row r="12" ht="33.75" spans="1:2">
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>52</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>-360</v>
       </c>
     </row>
-    <row r="13" ht="33.75" spans="1:2">
+    <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>-2693</v>
       </c>
     </row>
-    <row r="14" ht="33.75" spans="1:2">
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
fixed: combaine with some excluded elements to stats into file.
</commit_message>
<xml_diff>
--- a/original.xlsx
+++ b/original.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12380" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="12380" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>名称</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>张毅13316094116</t>
+  </si>
+  <si>
+    <t>李四12313131</t>
   </si>
 </sst>
 </file>
@@ -1644,8 +1647,8 @@
   <sheetPr/>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0234375" defaultRowHeight="16.8" outlineLevelCol="1"/>
@@ -1859,10 +1862,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0234375" defaultRowHeight="16.8" outlineLevelCol="1"/>
@@ -1983,6 +1986,14 @@
         <v>-1286</v>
       </c>
     </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <v>-200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>